<commit_message>
Cmabios Reporte, y anexamos Empresas aginadas
</commit_message>
<xml_diff>
--- a/recibos/bin/Debug/Archivos/reportenomina.xlsx
+++ b/recibos/bin/Debug/Archivos/reportenomina.xlsx
@@ -89,7 +89,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="94">
   <si>
     <t>SUBTOTAL</t>
   </si>
@@ -362,18 +362,26 @@
   </si>
   <si>
     <t>COMISION EXCEDENTE  (SINDICATO)</t>
+  </si>
+  <si>
+    <t>NOMBRE</t>
+  </si>
+  <si>
+    <t>PATRONA</t>
+  </si>
+  <si>
+    <t>CODIGO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="14">
+  <numFmts count="13">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
     <numFmt numFmtId="165" formatCode="0_ ;\-0\ "/>
-    <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="168" formatCode="_-* #,##0\ _$_-;\-* #,##0\ _$_-;_-* &quot;-&quot;\ _$_-;_-@_-"/>
     <numFmt numFmtId="169" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
@@ -808,7 +816,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="53">
+  <fills count="54">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1094,6 +1102,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2076,9 +2090,6 @@
     <xf numFmtId="44" fontId="44" fillId="0" borderId="0" xfId="280" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="46" fillId="50" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="280" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2095,9 +2106,6 @@
     <xf numFmtId="0" fontId="46" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="46" fillId="52" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="4" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2108,13 +2116,6 @@
     </xf>
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="38" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2137,6 +2138,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="59" fillId="0" borderId="0" xfId="194" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="53" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="53" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="53" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="46" fillId="50" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2169,6 +2177,12 @@
     </xf>
     <xf numFmtId="0" fontId="64" fillId="49" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="52" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="50" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="566">
@@ -3469,23 +3483,23 @@
   </sheetPr>
   <dimension ref="A1:Y66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" zoomScale="87" zoomScaleNormal="87" zoomScaleSheetLayoutView="120" workbookViewId="0">
-      <selection activeCell="S10" sqref="S10:V12"/>
+    <sheetView tabSelected="1" topLeftCell="D10" zoomScale="87" zoomScaleNormal="87" zoomScaleSheetLayoutView="120" workbookViewId="0">
+      <selection activeCell="S14" sqref="R14:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="34.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="43.42578125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="18.5703125" style="2" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" style="2" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" style="2" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="2" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11" style="2" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" style="2" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="13.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="18.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" style="1" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="16.85546875" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="18.5703125" style="1" customWidth="1"/>
     <col min="13" max="16" width="18.5703125" style="2" customWidth="1"/>
     <col min="17" max="18" width="18.5703125" style="1" customWidth="1"/>
     <col min="19" max="19" width="18.5703125" style="10" customWidth="1"/>
@@ -3497,8 +3511,8 @@
       <c r="A1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="93"/>
-      <c r="C1" s="92"/>
+      <c r="B1" s="91"/>
+      <c r="C1" s="90"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
@@ -3506,29 +3520,29 @@
       <c r="A2" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="92"/>
+      <c r="B2" s="90"/>
+      <c r="C2" s="90"/>
     </row>
     <row r="3" spans="1:25">
       <c r="A3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="113"/>
-      <c r="C3" s="113"/>
+      <c r="B3" s="111"/>
+      <c r="C3" s="111"/>
     </row>
     <row r="4" spans="1:25">
       <c r="A4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="92"/>
-      <c r="C4" s="92"/>
+      <c r="B4" s="90"/>
+      <c r="C4" s="90"/>
     </row>
     <row r="5" spans="1:25">
       <c r="A5" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="92"/>
-      <c r="C5" s="92"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
     </row>
     <row r="9" spans="1:25" ht="13.5">
       <c r="C9" s="1"/>
@@ -3591,133 +3605,129 @@
       <c r="U11" s="7"/>
       <c r="V11" s="7"/>
     </row>
-    <row r="12" spans="1:25" s="87" customFormat="1" ht="13.5">
-      <c r="A12" s="84">
+    <row r="12" spans="1:25" s="86" customFormat="1" ht="13.5">
+      <c r="A12" s="83">
         <f>B3</f>
         <v>0</v>
       </c>
-      <c r="B12" s="85"/>
-      <c r="C12" s="85"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="85"/>
-      <c r="F12" s="85"/>
-      <c r="G12" s="85"/>
-      <c r="H12" s="85"/>
-      <c r="I12" s="83"/>
-      <c r="J12" s="83"/>
-      <c r="K12" s="83"/>
-      <c r="L12" s="83"/>
-      <c r="M12" s="85"/>
-      <c r="N12" s="85"/>
-      <c r="O12" s="85"/>
-      <c r="P12" s="85"/>
-      <c r="Q12" s="86"/>
-      <c r="R12" s="86"/>
-      <c r="S12" s="86"/>
-      <c r="T12" s="86"/>
-      <c r="U12" s="86"/>
-      <c r="V12" s="86"/>
+      <c r="B12" s="84"/>
+      <c r="C12" s="84"/>
+      <c r="D12" s="84"/>
+      <c r="E12" s="84"/>
+      <c r="F12" s="84"/>
+      <c r="G12" s="84"/>
+      <c r="H12" s="84"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="84"/>
+      <c r="N12" s="84"/>
+      <c r="O12" s="84"/>
+      <c r="P12" s="84"/>
+      <c r="Q12" s="85"/>
+      <c r="R12" s="85"/>
+      <c r="S12" s="85"/>
+      <c r="T12" s="85"/>
+      <c r="U12" s="85"/>
+      <c r="V12" s="85"/>
     </row>
     <row r="13" spans="1:25" ht="30.75" customHeight="1">
-      <c r="A13" s="109" t="s">
+      <c r="A13" s="107" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="109" t="s">
+      <c r="B13" s="107" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="114" t="s">
+      <c r="C13" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="D13" s="109" t="s">
+      <c r="D13" s="107" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="109" t="s">
+      <c r="E13" s="107" t="s">
         <v>85</v>
       </c>
-      <c r="F13" s="109" t="s">
+      <c r="F13" s="107" t="s">
         <v>86</v>
       </c>
-      <c r="G13" s="110" t="s">
+      <c r="G13" s="108" t="s">
         <v>84</v>
       </c>
-      <c r="H13" s="110" t="s">
+      <c r="H13" s="108" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="88" t="s">
+      <c r="I13" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="J13" s="88" t="s">
+      <c r="J13" s="87" t="s">
         <v>87</v>
       </c>
-      <c r="K13" s="110" t="s">
+      <c r="K13" s="108" t="s">
         <v>81</v>
       </c>
-      <c r="L13" s="109" t="s">
+      <c r="L13" s="107" t="s">
         <v>16</v>
       </c>
-      <c r="M13" s="111" t="s">
+      <c r="M13" s="109" t="s">
         <v>33</v>
       </c>
-      <c r="N13" s="109" t="s">
+      <c r="N13" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="O13" s="110" t="s">
+      <c r="O13" s="108" t="s">
         <v>15</v>
       </c>
-      <c r="P13" s="110" t="s">
+      <c r="P13" s="108" t="s">
         <v>14</v>
       </c>
-      <c r="Q13" s="110" t="s">
+      <c r="Q13" s="108" t="s">
         <v>11</v>
       </c>
-      <c r="R13" s="82" t="s">
+      <c r="R13" s="81" t="s">
         <v>82</v>
       </c>
       <c r="S13" s="78" t="s">
         <v>90</v>
       </c>
-      <c r="T13" s="109" t="s">
+      <c r="T13" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="U13" s="112" t="s">
+      <c r="U13" s="110" t="s">
         <v>13</v>
       </c>
-      <c r="V13" s="109" t="s">
+      <c r="V13" s="107" t="s">
         <v>1</v>
       </c>
       <c r="W13" s="10"/>
     </row>
     <row r="14" spans="1:25" s="4" customFormat="1" ht="47.25" customHeight="1">
-      <c r="A14" s="109"/>
-      <c r="B14" s="109"/>
-      <c r="C14" s="114"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="109"/>
-      <c r="F14" s="109"/>
-      <c r="G14" s="110"/>
-      <c r="H14" s="110"/>
-      <c r="I14" s="88" t="s">
+      <c r="A14" s="107"/>
+      <c r="B14" s="107"/>
+      <c r="C14" s="112"/>
+      <c r="D14" s="107"/>
+      <c r="E14" s="107"/>
+      <c r="F14" s="107"/>
+      <c r="G14" s="108"/>
+      <c r="H14" s="108"/>
+      <c r="I14" s="87" t="s">
         <v>88</v>
       </c>
-      <c r="J14" s="88" t="s">
+      <c r="J14" s="87" t="s">
         <v>89</v>
       </c>
-      <c r="K14" s="110"/>
-      <c r="L14" s="109"/>
-      <c r="M14" s="111"/>
-      <c r="N14" s="109"/>
-      <c r="O14" s="110"/>
-      <c r="P14" s="110"/>
-      <c r="Q14" s="110"/>
-      <c r="R14" s="89">
-        <v>0.04</v>
-      </c>
-      <c r="S14" s="80">
-        <v>0.04</v>
-      </c>
-      <c r="T14" s="109"/>
-      <c r="U14" s="112"/>
-      <c r="V14" s="109"/>
+      <c r="K14" s="108"/>
+      <c r="L14" s="107"/>
+      <c r="M14" s="109"/>
+      <c r="N14" s="107"/>
+      <c r="O14" s="108"/>
+      <c r="P14" s="108"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="118"/>
+      <c r="S14" s="119"/>
+      <c r="T14" s="107"/>
+      <c r="U14" s="110"/>
+      <c r="V14" s="107"/>
       <c r="W14" s="11"/>
     </row>
     <row r="15" spans="1:25" s="15" customFormat="1" ht="14.25" customHeight="1">
@@ -3748,7 +3758,7 @@
       <c r="Y15" s="26"/>
     </row>
     <row r="16" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A16" s="90"/>
+      <c r="A16" s="88"/>
       <c r="B16" s="79"/>
       <c r="C16" s="47"/>
       <c r="D16" s="47"/>
@@ -3764,9 +3774,9 @@
       <c r="N16" s="12"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="81"/>
-      <c r="S16" s="81"/>
+      <c r="Q16" s="80"/>
+      <c r="R16" s="80"/>
+      <c r="S16" s="80"/>
       <c r="T16" s="12"/>
       <c r="U16" s="12"/>
       <c r="V16" s="12"/>
@@ -3775,7 +3785,7 @@
       <c r="Y16" s="26"/>
     </row>
     <row r="17" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A17" s="90"/>
+      <c r="A17" s="88"/>
       <c r="B17" s="79"/>
       <c r="C17" s="47"/>
       <c r="D17" s="47"/>
@@ -3791,9 +3801,9 @@
       <c r="N17" s="12"/>
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="81"/>
-      <c r="S17" s="81"/>
+      <c r="Q17" s="80"/>
+      <c r="R17" s="80"/>
+      <c r="S17" s="80"/>
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
       <c r="V17" s="12"/>
@@ -3802,7 +3812,7 @@
       <c r="Y17" s="26"/>
     </row>
     <row r="18" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A18" s="90"/>
+      <c r="A18" s="88"/>
       <c r="B18" s="79"/>
       <c r="C18" s="47"/>
       <c r="D18" s="47"/>
@@ -3818,9 +3828,9 @@
       <c r="N18" s="12"/>
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
-      <c r="Q18" s="81"/>
-      <c r="R18" s="81"/>
-      <c r="S18" s="81"/>
+      <c r="Q18" s="80"/>
+      <c r="R18" s="80"/>
+      <c r="S18" s="80"/>
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
       <c r="V18" s="12"/>
@@ -3829,7 +3839,7 @@
       <c r="Y18" s="26"/>
     </row>
     <row r="19" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A19" s="90"/>
+      <c r="A19" s="88"/>
       <c r="B19" s="79"/>
       <c r="C19" s="47"/>
       <c r="D19" s="47"/>
@@ -3845,9 +3855,9 @@
       <c r="N19" s="12"/>
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
-      <c r="Q19" s="81"/>
-      <c r="R19" s="81"/>
-      <c r="S19" s="81"/>
+      <c r="Q19" s="80"/>
+      <c r="R19" s="80"/>
+      <c r="S19" s="80"/>
       <c r="T19" s="12"/>
       <c r="U19" s="12"/>
       <c r="V19" s="12"/>
@@ -3856,7 +3866,7 @@
       <c r="Y19" s="26"/>
     </row>
     <row r="20" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A20" s="90"/>
+      <c r="A20" s="88"/>
       <c r="B20" s="79"/>
       <c r="C20" s="47"/>
       <c r="D20" s="47"/>
@@ -3872,9 +3882,9 @@
       <c r="N20" s="12"/>
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
-      <c r="Q20" s="81"/>
-      <c r="R20" s="81"/>
-      <c r="S20" s="81"/>
+      <c r="Q20" s="80"/>
+      <c r="R20" s="80"/>
+      <c r="S20" s="80"/>
       <c r="T20" s="12"/>
       <c r="U20" s="12"/>
       <c r="V20" s="12"/>
@@ -3883,7 +3893,7 @@
       <c r="Y20" s="26"/>
     </row>
     <row r="21" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A21" s="90"/>
+      <c r="A21" s="88"/>
       <c r="B21" s="79"/>
       <c r="C21" s="47"/>
       <c r="D21" s="47"/>
@@ -3899,9 +3909,9 @@
       <c r="N21" s="12"/>
       <c r="O21" s="12"/>
       <c r="P21" s="12"/>
-      <c r="Q21" s="81"/>
-      <c r="R21" s="81"/>
-      <c r="S21" s="81"/>
+      <c r="Q21" s="80"/>
+      <c r="R21" s="80"/>
+      <c r="S21" s="80"/>
       <c r="T21" s="12"/>
       <c r="U21" s="12"/>
       <c r="V21" s="12"/>
@@ -3910,7 +3920,7 @@
       <c r="Y21" s="26"/>
     </row>
     <row r="22" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A22" s="90"/>
+      <c r="A22" s="88"/>
       <c r="B22" s="79"/>
       <c r="C22" s="47"/>
       <c r="D22" s="47"/>
@@ -3926,9 +3936,9 @@
       <c r="N22" s="12"/>
       <c r="O22" s="12"/>
       <c r="P22" s="12"/>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="81"/>
-      <c r="S22" s="81"/>
+      <c r="Q22" s="80"/>
+      <c r="R22" s="80"/>
+      <c r="S22" s="80"/>
       <c r="T22" s="12"/>
       <c r="U22" s="12"/>
       <c r="V22" s="12"/>
@@ -3937,7 +3947,7 @@
       <c r="Y22" s="26"/>
     </row>
     <row r="23" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A23" s="90"/>
+      <c r="A23" s="88"/>
       <c r="B23" s="79"/>
       <c r="C23" s="47"/>
       <c r="D23" s="47"/>
@@ -3953,9 +3963,9 @@
       <c r="N23" s="12"/>
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
-      <c r="Q23" s="81"/>
-      <c r="R23" s="81"/>
-      <c r="S23" s="81"/>
+      <c r="Q23" s="80"/>
+      <c r="R23" s="80"/>
+      <c r="S23" s="80"/>
       <c r="T23" s="12"/>
       <c r="U23" s="12"/>
       <c r="V23" s="12"/>
@@ -3964,7 +3974,7 @@
       <c r="Y23" s="26"/>
     </row>
     <row r="24" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A24" s="90"/>
+      <c r="A24" s="88"/>
       <c r="B24" s="79"/>
       <c r="C24" s="47"/>
       <c r="D24" s="47"/>
@@ -3980,9 +3990,9 @@
       <c r="N24" s="12"/>
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
-      <c r="Q24" s="81"/>
-      <c r="R24" s="81"/>
-      <c r="S24" s="81"/>
+      <c r="Q24" s="80"/>
+      <c r="R24" s="80"/>
+      <c r="S24" s="80"/>
       <c r="T24" s="12"/>
       <c r="U24" s="12"/>
       <c r="V24" s="12"/>
@@ -3991,7 +4001,7 @@
       <c r="Y24" s="26"/>
     </row>
     <row r="25" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A25" s="90"/>
+      <c r="A25" s="88"/>
       <c r="B25" s="79"/>
       <c r="C25" s="47"/>
       <c r="D25" s="47"/>
@@ -4007,9 +4017,9 @@
       <c r="N25" s="12"/>
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
-      <c r="Q25" s="81"/>
-      <c r="R25" s="81"/>
-      <c r="S25" s="81"/>
+      <c r="Q25" s="80"/>
+      <c r="R25" s="80"/>
+      <c r="S25" s="80"/>
       <c r="T25" s="12"/>
       <c r="U25" s="12"/>
       <c r="V25" s="12"/>
@@ -4018,7 +4028,7 @@
       <c r="Y25" s="26"/>
     </row>
     <row r="26" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A26" s="90"/>
+      <c r="A26" s="88"/>
       <c r="B26" s="79"/>
       <c r="C26" s="47"/>
       <c r="D26" s="47"/>
@@ -4034,9 +4044,9 @@
       <c r="N26" s="12"/>
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
-      <c r="Q26" s="81"/>
-      <c r="R26" s="81"/>
-      <c r="S26" s="81"/>
+      <c r="Q26" s="80"/>
+      <c r="R26" s="80"/>
+      <c r="S26" s="80"/>
       <c r="T26" s="12"/>
       <c r="U26" s="12"/>
       <c r="V26" s="12"/>
@@ -4045,7 +4055,7 @@
       <c r="Y26" s="26"/>
     </row>
     <row r="27" spans="1:25" s="15" customFormat="1" ht="13.5">
-      <c r="A27" s="90"/>
+      <c r="A27" s="88"/>
       <c r="B27" s="79"/>
       <c r="C27" s="47"/>
       <c r="D27" s="47"/>
@@ -4061,9 +4071,9 @@
       <c r="N27" s="12"/>
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
-      <c r="Q27" s="81"/>
-      <c r="R27" s="81"/>
-      <c r="S27" s="81"/>
+      <c r="Q27" s="80"/>
+      <c r="R27" s="80"/>
+      <c r="S27" s="80"/>
       <c r="T27" s="12"/>
       <c r="U27" s="12"/>
       <c r="V27" s="12"/>
@@ -4099,29 +4109,29 @@
     </row>
     <row r="29" spans="1:25" s="15" customFormat="1" ht="13.5">
       <c r="A29" s="71"/>
-      <c r="B29" s="107"/>
-      <c r="C29" s="107"/>
-      <c r="D29" s="107"/>
-      <c r="E29" s="107"/>
-      <c r="F29" s="107"/>
-      <c r="G29" s="107"/>
-      <c r="H29" s="107"/>
-      <c r="I29" s="107"/>
-      <c r="J29" s="107"/>
-      <c r="K29" s="107"/>
-      <c r="L29" s="107"/>
-      <c r="M29" s="107"/>
-      <c r="N29" s="107"/>
-      <c r="O29" s="107"/>
-      <c r="P29" s="107"/>
-      <c r="Q29" s="107"/>
-      <c r="R29" s="107"/>
-      <c r="S29" s="107"/>
-      <c r="T29" s="107"/>
-      <c r="U29" s="107"/>
-      <c r="V29" s="107"/>
+      <c r="B29" s="102"/>
+      <c r="C29" s="102"/>
+      <c r="D29" s="102"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="102"/>
+      <c r="I29" s="102"/>
+      <c r="J29" s="102"/>
+      <c r="K29" s="102"/>
+      <c r="L29" s="102"/>
+      <c r="M29" s="102"/>
+      <c r="N29" s="102"/>
+      <c r="O29" s="102"/>
+      <c r="P29" s="102"/>
+      <c r="Q29" s="102"/>
+      <c r="R29" s="102"/>
+      <c r="S29" s="102"/>
+      <c r="T29" s="102"/>
+      <c r="U29" s="102"/>
+      <c r="V29" s="102"/>
       <c r="W29" s="72"/>
-      <c r="X29" s="108"/>
+      <c r="X29" s="103"/>
       <c r="Y29" s="26"/>
     </row>
     <row r="30" spans="1:25" s="17" customFormat="1" ht="13.5">
@@ -5163,48 +5173,48 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="12.75" customHeight="1">
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="115" t="s">
+      <c r="C3" s="113" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="115" t="s">
+      <c r="D3" s="113" t="s">
         <v>20</v>
       </c>
       <c r="E3" s="48"/>
-      <c r="F3" s="115" t="s">
+      <c r="F3" s="113" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="115" t="s">
+      <c r="G3" s="113" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="115" t="s">
+      <c r="H3" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="115" t="s">
+      <c r="I3" s="113" t="s">
         <v>33</v>
       </c>
       <c r="J3" s="28"/>
       <c r="K3" s="28"/>
-      <c r="L3" s="116"/>
+      <c r="L3" s="114"/>
     </row>
     <row r="4" spans="2:12" ht="12.75" customHeight="1">
-      <c r="B4" s="115"/>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
+      <c r="B4" s="113"/>
+      <c r="C4" s="113"/>
+      <c r="D4" s="113"/>
       <c r="E4" s="48"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="113"/>
+      <c r="H4" s="113"/>
+      <c r="I4" s="113"/>
       <c r="J4" s="28" t="s">
         <v>22</v>
       </c>
       <c r="K4" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="116"/>
+      <c r="L4" s="114"/>
     </row>
     <row r="5" spans="2:12" ht="15.75">
       <c r="B5" s="30" t="s">
@@ -5324,187 +5334,213 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:G19"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="9" max="9" width="26.42578125" customWidth="1"/>
-    <col min="10" max="10" width="21.7109375" customWidth="1"/>
-    <col min="11" max="11" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="48" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="21" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="26.42578125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="48" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
-      <c r="I1" s="33"/>
+    <row r="1" spans="1:11">
       <c r="J1" s="33"/>
-    </row>
-    <row r="2" spans="1:10">
+      <c r="K1" s="33"/>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="46"/>
-      <c r="B2" s="94"/>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
-      <c r="E2" s="95"/>
-      <c r="F2" s="95"/>
-      <c r="G2" s="95"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="B3" s="94"/>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="B4" s="96"/>
-      <c r="C4" s="96"/>
-      <c r="D4" s="97"/>
-      <c r="E4" s="97"/>
-      <c r="F4" s="98"/>
-      <c r="G4" s="96"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="B5" s="99"/>
-      <c r="C5" s="100"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="100"/>
-      <c r="F5" s="101"/>
-      <c r="G5" s="101"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="B6" s="99"/>
-      <c r="C6" s="100"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="100"/>
-      <c r="F6" s="101"/>
-      <c r="G6" s="101"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7" s="99"/>
-      <c r="C7" s="100"/>
-      <c r="D7" s="100"/>
-      <c r="E7" s="100"/>
-      <c r="F7" s="101"/>
-      <c r="G7" s="101"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" s="99"/>
-      <c r="C8" s="100"/>
-      <c r="D8" s="100"/>
-      <c r="E8" s="100"/>
-      <c r="F8" s="101"/>
-      <c r="G8" s="101"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="B9" s="99"/>
-      <c r="C9" s="100"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="100"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="B10" s="99"/>
-      <c r="C10" s="100"/>
-      <c r="D10" s="100"/>
-      <c r="E10" s="100"/>
-      <c r="F10" s="101"/>
-      <c r="G10" s="101"/>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="B11" s="99"/>
-      <c r="C11" s="100"/>
-      <c r="D11" s="100"/>
-      <c r="E11" s="100"/>
-      <c r="F11" s="101"/>
-      <c r="G11" s="101"/>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="B12" s="99"/>
-      <c r="C12" s="100"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="100"/>
-      <c r="F12" s="101"/>
-      <c r="G12" s="101"/>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="B13" s="99"/>
-      <c r="C13" s="100"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="100"/>
-      <c r="F13" s="101"/>
-      <c r="G13" s="101"/>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="B14" s="99"/>
-      <c r="C14" s="100"/>
-      <c r="D14" s="103"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="101"/>
-      <c r="G14" s="101"/>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="B15" s="99"/>
-      <c r="C15" s="100"/>
-      <c r="D15" s="103"/>
-      <c r="E15" s="100"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="101"/>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="B16" s="99"/>
-      <c r="C16" s="104"/>
-      <c r="D16" s="103"/>
-      <c r="E16" s="105"/>
-      <c r="F16" s="101"/>
-      <c r="G16" s="101"/>
-    </row>
-    <row r="17" spans="2:8">
-      <c r="B17" s="99"/>
-      <c r="C17" s="104"/>
-      <c r="D17" s="103"/>
-      <c r="E17" s="105"/>
-      <c r="F17" s="101"/>
-      <c r="G17" s="101"/>
-    </row>
-    <row r="18" spans="2:8">
-      <c r="B18" s="95"/>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
-      <c r="F18" s="95"/>
-      <c r="G18" s="95"/>
-    </row>
-    <row r="19" spans="2:8">
-      <c r="B19" s="95"/>
-      <c r="C19" s="95"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="94"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="91"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="92"/>
+      <c r="D2" s="93"/>
+      <c r="E2" s="93"/>
+      <c r="F2" s="93"/>
+      <c r="G2" s="93"/>
+      <c r="H2" s="93"/>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="C3" s="92"/>
+      <c r="D3" s="93"/>
+      <c r="E3" s="93"/>
+      <c r="F3" s="93"/>
+      <c r="G3" s="93"/>
+      <c r="H3" s="93"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="B4" s="104" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="104" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="105" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="105" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="106" t="s">
+        <v>92</v>
+      </c>
+      <c r="H4" s="104" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="105" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="105" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="104" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="C5" s="94"/>
+      <c r="D5" s="95"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="C6" s="94"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="96"/>
+      <c r="H6" s="96"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="C7" s="94"/>
+      <c r="D7" s="95"/>
+      <c r="E7" s="95"/>
+      <c r="F7" s="95"/>
+      <c r="G7" s="96"/>
+      <c r="H7" s="96"/>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="C8" s="94"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="95"/>
+      <c r="F8" s="95"/>
+      <c r="G8" s="96"/>
+      <c r="H8" s="96"/>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="C9" s="94"/>
+      <c r="D9" s="95"/>
+      <c r="E9" s="95"/>
+      <c r="F9" s="95"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="C10" s="94"/>
+      <c r="D10" s="95"/>
+      <c r="E10" s="95"/>
+      <c r="F10" s="95"/>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="C11" s="94"/>
+      <c r="D11" s="95"/>
+      <c r="E11" s="95"/>
+      <c r="F11" s="95"/>
+      <c r="G11" s="96"/>
+      <c r="H11" s="96"/>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="C12" s="94"/>
+      <c r="D12" s="95"/>
+      <c r="E12" s="97"/>
+      <c r="F12" s="95"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="C13" s="94"/>
+      <c r="D13" s="95"/>
+      <c r="E13" s="95"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="96"/>
+      <c r="H13" s="96"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="C14" s="94"/>
+      <c r="D14" s="95"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="95"/>
+      <c r="G14" s="96"/>
+      <c r="H14" s="96"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="C15" s="94"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="96"/>
+      <c r="H15" s="96"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="C16" s="94"/>
+      <c r="D16" s="99"/>
+      <c r="E16" s="98"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="96"/>
+      <c r="H16" s="96"/>
+    </row>
+    <row r="17" spans="3:9">
+      <c r="C17" s="94"/>
+      <c r="D17" s="99"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="100"/>
+      <c r="G17" s="96"/>
+      <c r="H17" s="96"/>
+    </row>
+    <row r="18" spans="3:9">
+      <c r="C18" s="93"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="99"/>
+      <c r="F18" s="99"/>
+      <c r="G18" s="93"/>
+      <c r="H18" s="93"/>
+    </row>
+    <row r="19" spans="3:9">
+      <c r="C19" s="93"/>
+      <c r="D19" s="93"/>
+      <c r="E19" s="93"/>
+      <c r="F19" s="92"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="101"/>
+      <c r="I19" s="89"/>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="D5:D9" name="Rango1"/>
-    <protectedRange sqref="E5:E7" name="Rango1_5_1"/>
-    <protectedRange sqref="D10:D12" name="Rango1_4_1"/>
-    <protectedRange sqref="C9" name="Rango1_1"/>
-    <protectedRange sqref="C5:C7" name="Rango1_5_4"/>
-    <protectedRange sqref="C10:C12" name="Rango1_5_4_1"/>
+    <protectedRange sqref="E5:E9" name="Rango1"/>
+    <protectedRange sqref="F5:F7" name="Rango1_5_1"/>
+    <protectedRange sqref="E10:E12" name="Rango1_4_1"/>
+    <protectedRange sqref="D9" name="Rango1_1"/>
+    <protectedRange sqref="D5:D7" name="Rango1_5_4"/>
+    <protectedRange sqref="D10:D12" name="Rango1_5_4_1"/>
   </protectedRanges>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="landscape" r:id="rId1"/>
@@ -5526,20 +5562,20 @@
   </cols>
   <sheetData>
     <row r="3" spans="5:7" ht="12.75" customHeight="1">
-      <c r="E3" s="115" t="s">
+      <c r="E3" s="113" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="115" t="s">
+      <c r="F3" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="115" t="s">
+      <c r="G3" s="113" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="4" spans="5:7" ht="12.75" customHeight="1">
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
+      <c r="E4" s="113"/>
+      <c r="F4" s="113"/>
+      <c r="G4" s="113"/>
     </row>
     <row r="6" spans="5:7" ht="12.75" customHeight="1">
       <c r="F6" s="32"/>
@@ -5789,10 +5825,10 @@
         <v>76</v>
       </c>
       <c r="AD2" s="62"/>
-      <c r="AE2" s="117"/>
-      <c r="AF2" s="118"/>
-      <c r="AG2" s="118"/>
-      <c r="AH2" s="119"/>
+      <c r="AE2" s="115"/>
+      <c r="AF2" s="116"/>
+      <c r="AG2" s="116"/>
+      <c r="AH2" s="117"/>
       <c r="AI2" s="69"/>
       <c r="AJ2" s="69"/>
       <c r="AK2" s="69"/>

</xml_diff>